<commit_message>
updated agenda to reflect recent changes
</commit_message>
<xml_diff>
--- a/admin/Agenda_4days_cleaned.xlsx
+++ b/admin/Agenda_4days_cleaned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C5261232\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d051945\gitHub\slvi\docker-k8s-training\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97AFD910-EF3D-4596-97BB-43D9FF37050D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D66EF0-5BA5-4E18-8FE6-F896198EA526}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33828" yWindow="1368" windowWidth="33600" windowHeight="5460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33825" yWindow="1365" windowWidth="33600" windowHeight="5460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day1" sheetId="29" r:id="rId1"/>
@@ -19,13 +19,18 @@
     <sheet name="Day 4" sheetId="32" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Day 2'!$B$9:$M$30</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Day 3'!$B$9:$M$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Day 2'!$B$9:$M$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Day 3'!$B$9:$M$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Day 4'!$B$9:$M$31</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Day1'!$B$9:$M$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Day1'!$B$9:$M$32</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
   <si>
     <t>Meeting Information:</t>
   </si>
@@ -139,12 +144,6 @@
     <t>Exercise 4: Expose your application</t>
   </si>
   <si>
-    <t>Exercise 6: ConfigMaps and secrets</t>
-  </si>
-  <si>
-    <t>Exercise Optional: Ingress</t>
-  </si>
-  <si>
     <t>Exercise 7: Statefulsets</t>
   </si>
   <si>
@@ -205,12 +204,6 @@
     <t>Exercise #2 – Ports and volumes</t>
   </si>
   <si>
-    <t>Exercise #3 – Images</t>
-  </si>
-  <si>
-    <t>Exercise #4 &amp; #5 – Docker files</t>
-  </si>
-  <si>
     <t>Presentation: Introduction to Kubernetes (K00)</t>
   </si>
   <si>
@@ -244,27 +237,15 @@
     <t>Presentation: Persistence (K05)</t>
   </si>
   <si>
-    <t>Presentation troubleshooting (K06)</t>
-  </si>
-  <si>
-    <t>Presentation: Config maps and secrets (K07)</t>
-  </si>
-  <si>
     <t>Feedback Day 3</t>
   </si>
   <si>
     <t>Optional Exercise 5: Create Helm chart for Ads</t>
   </si>
   <si>
-    <t>Presentation: Further entities (K08)</t>
-  </si>
-  <si>
     <t>Presentation: Helm (K12)</t>
   </si>
   <si>
-    <t>Presentation: Administration (2) (K11)</t>
-  </si>
-  <si>
     <t>Presentation: Administration (K11)</t>
   </si>
   <si>
@@ -290,6 +271,27 @@
   </si>
   <si>
     <t>Presentation: Why &amp; How</t>
+  </si>
+  <si>
+    <t>Exercise #3 &amp; #4 – Docker files</t>
+  </si>
+  <si>
+    <t>Presentation: Troubleshooting (K06)</t>
+  </si>
+  <si>
+    <t>Presentation: ConfigMaps &amp; Secrets (K07)</t>
+  </si>
+  <si>
+    <t>Exercise 6: ConfigMaps &amp; Secrets</t>
+  </si>
+  <si>
+    <t>Exercise: Ingress</t>
+  </si>
+  <si>
+    <t>Presentation: Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recap Helm + Exercise 9+10: Helm </t>
   </si>
 </sst>
 </file>
@@ -597,7 +599,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -652,34 +654,16 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -696,12 +680,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -728,19 +706,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1137,31 +1106,31 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:T36"/>
+  <dimension ref="B1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="2.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="2.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="27.140625" customWidth="1"/>
-    <col min="14" max="15" width="9.28515625" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" customWidth="1"/>
-    <col min="17" max="251" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="13" max="13" width="27.1640625" customWidth="1"/>
+    <col min="14" max="15" width="9.33203125" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" customWidth="1"/>
+    <col min="17" max="251" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" s="1" customFormat="1" ht="14.4" hidden="1">
+    <row r="1" spans="2:20" s="1" customFormat="1" ht="15" hidden="1">
       <c r="G1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1174,25 +1143,25 @@
     </row>
     <row r="2" spans="2:20" ht="0.6" hidden="1" customHeight="1">
       <c r="E2" s="12"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="35"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="2:20" ht="0.6" hidden="1" customHeight="1">
       <c r="E3" s="12"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="8"/>
       <c r="K3" s="9">
         <v>0.375</v>
@@ -1200,7 +1169,7 @@
       <c r="L3" s="9">
         <v>0.70833333333333337</v>
       </c>
-      <c r="M3" s="36"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="2:20" s="2" customFormat="1" hidden="1">
       <c r="F4" s="3"/>
@@ -1252,9 +1221,9 @@
       <c r="L8" s="5"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="2:20" s="2" customFormat="1" ht="21">
+    <row r="9" spans="2:20" s="2" customFormat="1" ht="20.25">
       <c r="B9" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -1275,7 +1244,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="2:20" s="2" customFormat="1" ht="12.6" thickBot="1">
+    <row r="11" spans="2:20" s="2" customFormat="1" ht="12.75" thickBot="1">
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1296,15 +1265,15 @@
       <c r="E12" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="37" t="s">
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="31" t="s">
         <v>6</v>
       </c>
       <c r="M12" s="20" t="s">
@@ -1313,15 +1282,15 @@
     </row>
     <row r="13" spans="2:20" ht="24" customHeight="1">
       <c r="B13" s="14">
-        <f t="shared" ref="B13:B26" ca="1" si="0">F13</f>
+        <f t="shared" ref="B13:B27" ca="1" si="0">F13</f>
         <v>1</v>
       </c>
       <c r="C13" s="15">
-        <f t="shared" ref="C13:C26" ca="1" si="1">IF(E13="Select","",IF(AND(F13=1,E13&lt;&gt;"Select"),$K$3,OFFSET(C13,-1,1)))</f>
+        <f t="shared" ref="C13:C27" ca="1" si="1">IF(E13="Select","",IF(AND(F13=1,E13&lt;&gt;"Select"),$K$3,OFFSET(C13,-1,1)))</f>
         <v>0.375</v>
       </c>
       <c r="D13" s="15">
-        <f t="shared" ref="D13:D26" ca="1" si="2">IF(ISERROR(E13+C13),"",E13+C13)</f>
+        <f t="shared" ref="D13:D27" ca="1" si="2">IF(ISERROR(E13+C13),"",E13+C13)</f>
         <v>0.41666666666666669</v>
       </c>
       <c r="E13" s="16">
@@ -1331,20 +1300,20 @@
         <f t="shared" ref="F13:F23" ca="1" si="3">ROW()-ROW(OFFSET(F13,-1,))+IF(ISERROR(OFFSET(F13,-1,)*1),0,OFFSET(F13,-1,))</f>
         <v>1</v>
       </c>
-      <c r="G13" s="62" t="s">
+      <c r="G13" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="38" t="s">
-        <v>24</v>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="32" t="s">
+        <v>22</v>
       </c>
       <c r="M13" s="17"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="48"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="40"/>
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
@@ -1361,27 +1330,27 @@
       </c>
       <c r="D14" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.4236111111111111</v>
+        <v>0.43055555555555558</v>
       </c>
       <c r="E14" s="16">
-        <v>6.9444444444444441E-3</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="F14" s="17">
         <f ca="1">ROW()-ROW(OFFSET(F14,-1,))+IF(ISERROR(OFFSET(F14,-1,)*1),0,OFFSET(F14,-1,))</f>
         <v>2</v>
       </c>
-      <c r="G14" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="56"/>
+      <c r="G14" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="46"/>
       <c r="M14" s="17"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="48"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="40"/>
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
@@ -1394,31 +1363,31 @@
       </c>
       <c r="C15" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4236111111111111</v>
+        <v>0.43055555555555558</v>
       </c>
       <c r="D15" s="15">
         <f t="shared" ca="1" si="2"/>
         <v>0.4375</v>
       </c>
       <c r="E15" s="16">
-        <v>1.3888888888888888E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="F15" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
-      <c r="G15" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="53"/>
+      <c r="G15" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="45"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="47"/>
-      <c r="P15" s="48"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="40"/>
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
@@ -1435,27 +1404,27 @@
       </c>
       <c r="D16" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.46875</v>
+        <v>0.46527777777777779</v>
       </c>
       <c r="E16" s="16">
-        <v>3.125E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="F16" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>4</v>
       </c>
-      <c r="G16" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="25"/>
+      <c r="G16" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="53"/>
       <c r="L16" s="23"/>
       <c r="M16" s="17"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="49"/>
-      <c r="P16" s="48"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="40"/>
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
@@ -1468,31 +1437,31 @@
       </c>
       <c r="C17" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46875</v>
+        <v>0.46527777777777779</v>
       </c>
       <c r="D17" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.48958333333333331</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="E17" s="16">
-        <v>2.0833333333333332E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="F17" s="17">
         <f ca="1">ROW()-ROW(OFFSET(F17,-1,))+IF(ISERROR(OFFSET(F17,-1,)*1),0,OFFSET(F17,-1,))</f>
         <v>5</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="25"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="53"/>
       <c r="L17" s="23"/>
       <c r="M17" s="17"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="49"/>
-      <c r="P17" s="48"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="40"/>
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="22"/>
@@ -1505,31 +1474,31 @@
       </c>
       <c r="C18" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48958333333333331</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="D18" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.52083333333333326</v>
+        <v>0.50694444444444442</v>
       </c>
       <c r="E18" s="16">
-        <v>3.125E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="F18" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-      <c r="G18" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="25"/>
+      <c r="G18" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="53"/>
       <c r="L18" s="23"/>
       <c r="M18" s="17"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="48"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="40"/>
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
@@ -1542,11 +1511,11 @@
       </c>
       <c r="C19" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52083333333333326</v>
+        <v>0.50694444444444442</v>
       </c>
       <c r="D19" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.53124999999999989</v>
+        <v>0.51736111111111105</v>
       </c>
       <c r="E19" s="16">
         <v>1.0416666666666666E-2</v>
@@ -1555,18 +1524,18 @@
         <f ca="1">ROW()-ROW(OFFSET(F19,-1,))+IF(ISERROR(OFFSET(F19,-1,)*1),0,OFFSET(F19,-1,))</f>
         <v>7</v>
       </c>
-      <c r="G19" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="38"/>
+      <c r="G19" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="32"/>
       <c r="M19" s="17"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="49"/>
-      <c r="P19" s="48"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="40"/>
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
@@ -1579,11 +1548,11 @@
       </c>
       <c r="C20" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53124999999999989</v>
+        <v>0.51736111111111105</v>
       </c>
       <c r="D20" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.57291666666666652</v>
+        <v>0.55902777777777768</v>
       </c>
       <c r="E20" s="16">
         <v>4.1666666666666664E-2</v>
@@ -1592,18 +1561,18 @@
         <f t="shared" ca="1" si="3"/>
         <v>8</v>
       </c>
-      <c r="G20" s="27" t="s">
+      <c r="G20" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="27"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="25"/>
       <c r="M20" s="17"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="48"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="40"/>
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
       <c r="S20" s="22"/>
@@ -1616,31 +1585,31 @@
       </c>
       <c r="C21" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.57291666666666652</v>
+        <v>0.55902777777777768</v>
       </c>
       <c r="D21" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.60416666666666652</v>
+        <v>0.57986111111111105</v>
       </c>
       <c r="E21" s="16">
-        <v>3.125E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F21" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>9</v>
       </c>
-      <c r="G21" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="38"/>
+      <c r="G21" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="32"/>
       <c r="M21" s="17"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
@@ -1653,31 +1622,31 @@
       </c>
       <c r="C22" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60416666666666652</v>
+        <v>0.57986111111111105</v>
       </c>
       <c r="D22" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.62499999999999989</v>
+        <v>0.59374999999999989</v>
       </c>
       <c r="E22" s="16">
-        <v>2.0833333333333332E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="F22" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>10</v>
       </c>
-      <c r="G22" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="38"/>
+      <c r="G22" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="32"/>
       <c r="M22" s="17"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="48"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="40"/>
       <c r="Q22" s="22"/>
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
@@ -1690,31 +1659,31 @@
       </c>
       <c r="C23" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62499999999999989</v>
+        <v>0.59374999999999989</v>
       </c>
       <c r="D23" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.64930555555555547</v>
+        <v>0.61458333333333326</v>
       </c>
       <c r="E23" s="16">
-        <v>2.4305555555555556E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F23" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>11</v>
       </c>
-      <c r="G23" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="38"/>
+      <c r="G23" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="32"/>
       <c r="M23" s="17"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="48"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="40"/>
       <c r="Q23" s="22"/>
       <c r="R23" s="22"/>
       <c r="S23" s="22"/>
@@ -1727,31 +1696,31 @@
       </c>
       <c r="C24" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64930555555555547</v>
+        <v>0.61458333333333326</v>
       </c>
       <c r="D24" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.67708333333333326</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="E24" s="16">
-        <v>2.7777777777777776E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F24" s="17">
-        <f ca="1">ROW()-ROW(OFFSET(F24,-1,))+IF(ISERROR(OFFSET(F24,-1,)*1),0,OFFSET(F24,-1,))</f>
+        <f t="shared" ref="F24:F29" ca="1" si="4">ROW()-ROW(OFFSET(F24,-1,))+IF(ISERROR(OFFSET(F24,-1,)*1),0,OFFSET(F24,-1,))</f>
         <v>12</v>
       </c>
-      <c r="G24" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="38"/>
+      <c r="G24" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="32"/>
       <c r="M24" s="17"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="48"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="40"/>
       <c r="Q24" s="22"/>
       <c r="R24" s="22"/>
       <c r="S24" s="22"/>
@@ -1764,31 +1733,31 @@
       </c>
       <c r="C25" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67708333333333326</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="D25" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.6909722222222221</v>
+        <v>0.65625</v>
       </c>
       <c r="E25" s="16">
-        <v>1.3888888888888888E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F25" s="17">
-        <f ca="1">ROW()-ROW(OFFSET(F25,-1,))+IF(ISERROR(OFFSET(F25,-1,)*1),0,OFFSET(F25,-1,))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>13</v>
       </c>
-      <c r="G25" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="27"/>
+      <c r="G25" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="25"/>
       <c r="M25" s="17"/>
-      <c r="N25" s="50"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="48"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="40"/>
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="22"/>
@@ -1796,36 +1765,36 @@
     </row>
     <row r="26" spans="2:20" ht="24" customHeight="1">
       <c r="B26" s="14">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="B26" ca="1" si="5">F26</f>
         <v>14</v>
       </c>
       <c r="C26" s="15">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.6909722222222221</v>
+        <f t="shared" ref="C26" ca="1" si="6">IF(E26="Select","",IF(AND(F26=1,E26&lt;&gt;"Select"),$K$3,OFFSET(C26,-1,1)))</f>
+        <v>0.65625</v>
       </c>
       <c r="D26" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.70138888888888873</v>
+        <f t="shared" ref="D26" ca="1" si="7">IF(ISERROR(E26+C26),"",E26+C26)</f>
+        <v>0.66319444444444442</v>
       </c>
       <c r="E26" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="F26" s="17">
-        <f ca="1">ROW()-ROW(OFFSET(F26,-1,))+IF(ISERROR(OFFSET(F26,-1,)*1),0,OFFSET(F26,-1,))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>14</v>
       </c>
-      <c r="G26" s="62" t="s">
-        <v>42</v>
-      </c>
-      <c r="H26" s="63"/>
-      <c r="I26" s="63"/>
-      <c r="J26" s="63"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="27"/>
+      <c r="G26" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="50"/>
       <c r="M26" s="17"/>
-      <c r="N26" s="50"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="48"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="40"/>
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="22"/>
@@ -1833,88 +1802,173 @@
     </row>
     <row r="27" spans="2:20" ht="24" customHeight="1">
       <c r="B27" s="14">
-        <f t="shared" ref="B27" ca="1" si="4">F27</f>
+        <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
       <c r="C27" s="15">
-        <f t="shared" ref="C27" ca="1" si="5">IF(E27="Select","",IF(AND(F27=1,E27&lt;&gt;"Select"),$K$3,OFFSET(C27,-1,1)))</f>
-        <v>0.70138888888888873</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.66319444444444442</v>
       </c>
       <c r="D27" s="15">
-        <f t="shared" ref="D27" ca="1" si="6">IF(ISERROR(E27+C27),"",E27+C27)</f>
-        <v>0.70833333333333315</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.68402777777777779</v>
       </c>
       <c r="E27" s="16">
-        <v>6.9444444444444441E-3</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F27" s="17">
-        <f ca="1">ROW()-ROW(OFFSET(F27,-1,))+IF(ISERROR(OFFSET(F27,-1,)*1),0,OFFSET(F27,-1,))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>15</v>
       </c>
-      <c r="G27" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="38"/>
+      <c r="G27" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="25"/>
       <c r="M27" s="17"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="50"/>
-      <c r="P27" s="48"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="40"/>
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="22"/>
       <c r="T27" s="22"/>
     </row>
-    <row r="28" spans="2:20" ht="22.5" customHeight="1">
-      <c r="E28" s="18">
-        <f>SUM(E13:E27)</f>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="31" spans="2:20" ht="15.6">
-      <c r="B31" s="13" t="s">
+    <row r="28" spans="2:20" ht="24" customHeight="1">
+      <c r="B28" s="14">
+        <f t="shared" ref="B28" ca="1" si="8">F28</f>
+        <v>16</v>
+      </c>
+      <c r="C28" s="15">
+        <f t="shared" ref="C28" ca="1" si="9">IF(E28="Select","",IF(AND(F28=1,E28&lt;&gt;"Select"),$K$3,OFFSET(C28,-1,1)))</f>
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="D28" s="15">
+        <f t="shared" ref="D28" ca="1" si="10">IF(ISERROR(E28+C28),"",E28+C28)</f>
+        <v>0.70138888888888895</v>
+      </c>
+      <c r="E28" s="16">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F28" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="G28" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+    </row>
+    <row r="29" spans="2:20" ht="24" customHeight="1">
+      <c r="B29" s="14">
+        <f t="shared" ref="B29" ca="1" si="11">F29</f>
+        <v>17</v>
+      </c>
+      <c r="C29" s="15">
+        <f t="shared" ref="C29" ca="1" si="12">IF(E29="Select","",IF(AND(F29=1,E29&lt;&gt;"Select"),$K$3,OFFSET(C29,-1,1)))</f>
+        <v>0.70138888888888895</v>
+      </c>
+      <c r="D29" s="15">
+        <f t="shared" ref="D29" ca="1" si="13">IF(ISERROR(E29+C29),"",E29+C29)</f>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E29" s="16">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="F29" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="G29" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+    </row>
+    <row r="30" spans="2:20" ht="22.5" customHeight="1">
+      <c r="E30" s="18">
+        <f>SUM(E13:E28)</f>
+        <v>0.32638888888888878</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="15.75">
+      <c r="B33" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="15.6">
-      <c r="B34" s="2"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="2:4" ht="15.6">
-      <c r="B35" s="2"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="2:4" ht="14.4">
+    <row r="36" spans="2:4" ht="15.75">
       <c r="B36" s="2"/>
-      <c r="C36" s="46"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="2"/>
     </row>
+    <row r="37" spans="2:4" ht="15.75">
+      <c r="B37" s="2"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="2:4" ht="15">
+      <c r="B38" s="2"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="G26:K26"/>
+  <mergeCells count="20">
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="F12:K12"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G29:K29"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="G25:K25"/>
     <mergeCell ref="G22:K22"/>
     <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G23:K23"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="E28">
+  <conditionalFormatting sqref="E30">
     <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter time as H:MM:SS (update AM/PM as necessary)." sqref="K3:L11" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E27" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E29" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"0:00, 0:05, 0:10, 0:15, 0:20, 0:25, 0:30, 0:35, 0:40, 0:45, 0:50, 0:55, 1:00, 1:15, 1:30"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1928,29 +1982,29 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:T36"/>
+  <dimension ref="B1:T39"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView topLeftCell="B9" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="2.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="2.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" customWidth="1"/>
-    <col min="14" max="251" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" customWidth="1"/>
+    <col min="14" max="251" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" s="1" customFormat="1" ht="14.4" hidden="1">
+    <row r="1" spans="2:20" s="1" customFormat="1" ht="15" hidden="1">
       <c r="G1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1963,25 +2017,25 @@
     </row>
     <row r="2" spans="2:20" ht="12" hidden="1" customHeight="1">
       <c r="E2" s="12"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="35"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="2:20" ht="12" hidden="1" customHeight="1">
       <c r="E3" s="12"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="8"/>
       <c r="K3" s="9">
         <v>0.375</v>
@@ -1989,7 +2043,7 @@
       <c r="L3" s="9">
         <v>0.70833333333333337</v>
       </c>
-      <c r="M3" s="36"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="2:20" s="2" customFormat="1" hidden="1">
       <c r="F4" s="3"/>
@@ -2041,9 +2095,9 @@
       <c r="L8" s="5"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="2:20" s="2" customFormat="1" ht="21">
+    <row r="9" spans="2:20" s="2" customFormat="1" ht="20.25">
       <c r="B9" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -2064,7 +2118,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="2:20" s="2" customFormat="1" ht="12.6" thickBot="1">
+    <row r="11" spans="2:20" s="2" customFormat="1" ht="12.75" thickBot="1">
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2085,15 +2139,15 @@
       <c r="E12" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="37" t="s">
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="31" t="s">
         <v>6</v>
       </c>
       <c r="M12" s="20" t="s">
@@ -2102,7 +2156,7 @@
     </row>
     <row r="13" spans="2:20" ht="24" customHeight="1">
       <c r="B13" s="14">
-        <f t="shared" ref="B13:B27" ca="1" si="0">F13</f>
+        <f t="shared" ref="B13:B30" ca="1" si="0">F13</f>
         <v>1</v>
       </c>
       <c r="C13" s="15">
@@ -2120,18 +2174,18 @@
         <f t="shared" ref="F13:F25" ca="1" si="2">ROW()-ROW(OFFSET(F13,-1,))+IF(ISERROR(OFFSET(F13,-1,)*1),0,OFFSET(F13,-1,))</f>
         <v>1</v>
       </c>
-      <c r="G13" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="38"/>
+      <c r="G13" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="32"/>
       <c r="M13" s="17"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="51"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="43"/>
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
@@ -2148,27 +2202,27 @@
       </c>
       <c r="D14" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39583333333333337</v>
+        <v>0.40625</v>
       </c>
       <c r="E14" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F14" s="17">
         <f ca="1">ROW()-ROW(OFFSET(F14,-1,))+IF(ISERROR(OFFSET(F14,-1,)*1),0,OFFSET(F14,-1,))</f>
         <v>2</v>
       </c>
-      <c r="G14" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="56"/>
+      <c r="G14" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="46"/>
       <c r="M14" s="17"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
@@ -2181,31 +2235,31 @@
       </c>
       <c r="C15" s="15">
         <f ca="1">IF(E15="Select","",IF(AND(F15=1,E15&lt;&gt;"Select"),'Day1'!$K$3,OFFSET(C15,-1,1)))</f>
-        <v>0.39583333333333337</v>
+        <v>0.40625</v>
       </c>
       <c r="D15" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44791666666666669</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="E15" s="16">
-        <v>5.2083333333333336E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="F15" s="17">
         <f ca="1">ROW()-ROW(OFFSET(F15,-1,))+IF(ISERROR(OFFSET(F15,-1,)*1),0,OFFSET(F15,-1,))</f>
         <v>3</v>
       </c>
-      <c r="G15" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="56"/>
+      <c r="G15" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="46"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
@@ -2218,11 +2272,11 @@
       </c>
       <c r="C16" s="15">
         <f t="shared" ref="C16:C26" ca="1" si="3">IF(E16="Select","",IF(AND(F16=1,E16&lt;&gt;"Select"),$K$3,OFFSET(C16,-1,1)))</f>
-        <v>0.44791666666666669</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D16" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4548611111111111</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E16" s="16">
         <v>6.9444444444444441E-3</v>
@@ -2231,18 +2285,18 @@
         <f ca="1">ROW()-ROW(OFFSET(F16,-1,))+IF(ISERROR(OFFSET(F16,-1,)*1),0,OFFSET(F16,-1,))</f>
         <v>4</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="31"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="27"/>
       <c r="M16" s="17"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="49"/>
-      <c r="P16" s="49"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
@@ -2255,31 +2309,31 @@
       </c>
       <c r="C17" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.4548611111111111</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="D17" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46527777777777779</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E17" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F17" s="17">
         <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
-      <c r="G17" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="31"/>
+      <c r="G17" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="27"/>
       <c r="M17" s="17"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="49"/>
-      <c r="P17" s="49"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="22"/>
@@ -2292,31 +2346,31 @@
       </c>
       <c r="C18" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.46527777777777779</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D18" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="E18" s="16">
-        <v>3.4722222222222224E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="F18" s="17">
         <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
-      <c r="G18" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="31"/>
+      <c r="G18" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="27"/>
       <c r="M18" s="17"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="49"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
@@ -2329,31 +2383,31 @@
       </c>
       <c r="C19" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.5</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="D19" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.51041666666666663</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="E19" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>2.4305555555555556E-2</v>
       </c>
       <c r="F19" s="17">
         <f t="shared" ca="1" si="2"/>
         <v>7</v>
       </c>
-      <c r="G19" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="38"/>
+      <c r="G19" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="32"/>
       <c r="M19" s="17"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="49"/>
-      <c r="P19" s="49"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
@@ -2366,31 +2420,31 @@
       </c>
       <c r="C20" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.51041666666666663</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="D20" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55208333333333326</v>
+        <v>0.50347222222222221</v>
       </c>
       <c r="E20" s="16">
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F20" s="17">
         <f ca="1">ROW()-ROW(OFFSET(F20,-1,))+IF(ISERROR(OFFSET(F20,-1,)*1),0,OFFSET(F20,-1,))</f>
         <v>8</v>
       </c>
-      <c r="G20" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="56"/>
+      <c r="G20" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="46"/>
       <c r="M20" s="17"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="49"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
       <c r="S20" s="22"/>
@@ -2403,31 +2457,31 @@
       </c>
       <c r="C21" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.55208333333333326</v>
+        <v>0.50347222222222221</v>
       </c>
       <c r="D21" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.57986111111111105</v>
+        <v>0.54513888888888884</v>
       </c>
       <c r="E21" s="16">
-        <v>2.7777777777777776E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F21" s="17">
         <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
-      <c r="G21" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="31"/>
+      <c r="G21" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="27"/>
       <c r="M21" s="17"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="49"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
@@ -2440,31 +2494,31 @@
       </c>
       <c r="C22" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.57986111111111105</v>
+        <v>0.54513888888888884</v>
       </c>
       <c r="D22" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60416666666666663</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="E22" s="16">
-        <v>2.4305555555555556E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="F22" s="17">
         <f t="shared" ca="1" si="2"/>
         <v>10</v>
       </c>
-      <c r="G22" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="38"/>
+      <c r="G22" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="32"/>
       <c r="M22" s="17"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="49"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
       <c r="Q22" s="22"/>
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
@@ -2477,31 +2531,31 @@
       </c>
       <c r="C23" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.60416666666666663</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="D23" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64583333333333326</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="E23" s="16">
-        <v>4.1666666666666664E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="F23" s="17">
         <f t="shared" ca="1" si="2"/>
         <v>11</v>
       </c>
-      <c r="G23" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="38"/>
+      <c r="G23" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="32"/>
       <c r="M23" s="17"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
       <c r="Q23" s="22"/>
       <c r="R23" s="22"/>
       <c r="S23" s="22"/>
@@ -2514,31 +2568,31 @@
       </c>
       <c r="C24" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.64583333333333326</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="D24" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="E24" s="16">
-        <v>2.0833333333333332E-2</v>
+        <v>2.4305555555555556E-2</v>
       </c>
       <c r="F24" s="17">
         <f t="shared" ca="1" si="2"/>
         <v>12</v>
       </c>
-      <c r="G24" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="38"/>
+      <c r="G24" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="32"/>
       <c r="M24" s="17"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="49"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
       <c r="Q24" s="22"/>
       <c r="R24" s="22"/>
       <c r="S24" s="22"/>
@@ -2551,11 +2605,11 @@
       </c>
       <c r="C25" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.66666666666666663</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="D25" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6875</v>
+        <v>0.63541666666666674</v>
       </c>
       <c r="E25" s="16">
         <v>2.0833333333333332E-2</v>
@@ -2564,18 +2618,18 @@
         <f t="shared" ca="1" si="2"/>
         <v>13</v>
       </c>
-      <c r="G25" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="31"/>
+      <c r="G25" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="27"/>
       <c r="M25" s="17"/>
-      <c r="N25" s="50"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="49"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="22"/>
@@ -2588,31 +2642,31 @@
       </c>
       <c r="C26" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6875</v>
+        <v>0.63541666666666674</v>
       </c>
       <c r="D26" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69791666666666663</v>
+        <v>0.64236111111111116</v>
       </c>
       <c r="E26" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="F26" s="17">
         <f ca="1">ROW()-ROW(OFFSET(F26,-1,))+IF(ISERROR(OFFSET(F26,-1,)*1),0,OFFSET(F26,-1,))</f>
         <v>14</v>
       </c>
-      <c r="G26" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="38"/>
+      <c r="G26" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="32"/>
       <c r="M26" s="17"/>
-      <c r="N26" s="50"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="49"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="22"/>
@@ -2620,16 +2674,16 @@
     </row>
     <row r="27" spans="2:20" ht="24" customHeight="1">
       <c r="B27" s="14">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="B27" ca="1" si="4">F27</f>
         <v>15</v>
       </c>
       <c r="C27" s="15">
-        <f t="shared" ref="C27" ca="1" si="4">IF(E27="Select","",IF(AND(F27=1,E27&lt;&gt;"Select"),$K$3,OFFSET(C27,-1,1)))</f>
-        <v>0.69791666666666663</v>
+        <f t="shared" ref="C27" ca="1" si="5">IF(E27="Select","",IF(AND(F27=1,E27&lt;&gt;"Select"),$K$3,OFFSET(C27,-1,1)))</f>
+        <v>0.64236111111111116</v>
       </c>
       <c r="D27" s="15">
-        <f t="shared" ref="D27" ca="1" si="5">IF(ISERROR(E27+C27),"",E27+C27)</f>
-        <v>0.70833333333333326</v>
+        <f t="shared" ref="D27" ca="1" si="6">IF(ISERROR(E27+C27),"",E27+C27)</f>
+        <v>0.65277777777777779</v>
       </c>
       <c r="E27" s="16">
         <v>1.0416666666666666E-2</v>
@@ -2638,62 +2692,186 @@
         <f ca="1">ROW()-ROW(OFFSET(F27,-1,))+IF(ISERROR(OFFSET(F27,-1,)*1),0,OFFSET(F27,-1,))</f>
         <v>15</v>
       </c>
-      <c r="G27" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="38"/>
+      <c r="G27" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="50"/>
       <c r="M27" s="17"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="50"/>
-      <c r="P27" s="51"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="22"/>
       <c r="T27" s="22"/>
     </row>
-    <row r="28" spans="2:20" ht="22.5" customHeight="1">
-      <c r="E28" s="18">
-        <f>SUM(E13:E27)</f>
+    <row r="28" spans="2:20" ht="24" customHeight="1">
+      <c r="B28" s="14">
+        <f t="shared" ref="B28" ca="1" si="7">F28</f>
+        <v>16</v>
+      </c>
+      <c r="C28" s="15">
+        <f t="shared" ref="C28" ca="1" si="8">IF(E28="Select","",IF(AND(F28=1,E28&lt;&gt;"Select"),$K$3,OFFSET(C28,-1,1)))</f>
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D28" s="15">
+        <f t="shared" ref="D28" ca="1" si="9">IF(ISERROR(E28+C28),"",E28+C28)</f>
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="E28" s="16">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="F28" s="17">
+        <f ca="1">ROW()-ROW(OFFSET(F28,-1,))+IF(ISERROR(OFFSET(F28,-1,)*1),0,OFFSET(F28,-1,))</f>
+        <v>16</v>
+      </c>
+      <c r="G28" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+    </row>
+    <row r="29" spans="2:20" ht="24" customHeight="1">
+      <c r="B29" s="14">
+        <f t="shared" ref="B29" ca="1" si="10">F29</f>
+        <v>17</v>
+      </c>
+      <c r="C29" s="15">
+        <f t="shared" ref="C29" ca="1" si="11">IF(E29="Select","",IF(AND(F29=1,E29&lt;&gt;"Select"),$K$3,OFFSET(C29,-1,1)))</f>
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D29" s="15">
+        <f t="shared" ref="D29" ca="1" si="12">IF(ISERROR(E29+C29),"",E29+C29)</f>
+        <v>0.69791666666666674</v>
+      </c>
+      <c r="E29" s="16">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F29" s="17">
+        <f ca="1">ROW()-ROW(OFFSET(F29,-1,))+IF(ISERROR(OFFSET(F29,-1,)*1),0,OFFSET(F29,-1,))</f>
+        <v>17</v>
+      </c>
+      <c r="G29" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+    </row>
+    <row r="30" spans="2:20" ht="24" customHeight="1">
+      <c r="B30" s="14">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C30" s="15">
+        <f t="shared" ref="C30" ca="1" si="13">IF(E30="Select","",IF(AND(F30=1,E30&lt;&gt;"Select"),$K$3,OFFSET(C30,-1,1)))</f>
+        <v>0.69791666666666674</v>
+      </c>
+      <c r="D30" s="15">
+        <f t="shared" ref="D30" ca="1" si="14">IF(ISERROR(E30+C30),"",E30+C30)</f>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E30" s="16">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F30" s="17">
+        <f ca="1">ROW()-ROW(OFFSET(F30,-1,))+IF(ISERROR(OFFSET(F30,-1,)*1),0,OFFSET(F30,-1,))</f>
+        <v>18</v>
+      </c>
+      <c r="G30" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
+    </row>
+    <row r="31" spans="2:20" ht="22.5" customHeight="1">
+      <c r="E31" s="18">
+        <f>SUM(E13:E30)</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="15.6">
-      <c r="B31" s="13" t="s">
+    <row r="34" spans="2:3" ht="15.75">
+      <c r="B34" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="3:3" ht="15.6">
-      <c r="C34" s="44"/>
-    </row>
-    <row r="35" spans="3:3" ht="15.6">
-      <c r="C35" s="45"/>
-    </row>
-    <row r="36" spans="3:3" ht="14.4">
-      <c r="C36" s="46"/>
+    <row r="37" spans="2:3" ht="15.75">
+      <c r="C37" s="36"/>
+    </row>
+    <row r="38" spans="2:3" ht="15.75">
+      <c r="C38" s="37"/>
+    </row>
+    <row r="39" spans="2:3" ht="15">
+      <c r="C39" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="21">
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="F12:K12"/>
-    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G30:K30"/>
     <mergeCell ref="G24:K24"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G29:K29"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G26:K26"/>
     <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G28:K28"/>
   </mergeCells>
-  <conditionalFormatting sqref="E28">
+  <conditionalFormatting sqref="E31">
     <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter time as H:MM:SS (update AM/PM as necessary)." sqref="K3:L11" xr:uid="{A6668F6F-6387-429D-A96E-6340520C81CD}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E26 E27" xr:uid="{9553B08E-9F8B-4959-9B86-3BB907715C00}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E30" xr:uid="{9553B08E-9F8B-4959-9B86-3BB907715C00}">
       <formula1>"0:00, 0:05, 0:10, 0:15, 0:20, 0:25, 0:30, 0:35, 0:40, 0:45, 0:50, 0:55, 1:00, 1:15, 1:30"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2707,29 +2885,29 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:T41"/>
+  <dimension ref="B1:T36"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView topLeftCell="B11" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="2.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="2.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="14" max="251" width="9.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
+    <col min="14" max="251" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" s="1" customFormat="1" ht="14.4" hidden="1">
+    <row r="1" spans="2:20" s="1" customFormat="1" ht="15" hidden="1">
       <c r="G1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2742,25 +2920,25 @@
     </row>
     <row r="2" spans="2:20" ht="12" hidden="1" customHeight="1">
       <c r="E2" s="12"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="35"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="2:20" ht="12" hidden="1" customHeight="1">
       <c r="E3" s="12"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="8"/>
       <c r="K3" s="9">
         <v>0.375</v>
@@ -2768,7 +2946,7 @@
       <c r="L3" s="9">
         <v>0.70833333333333337</v>
       </c>
-      <c r="M3" s="36"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="2:20" s="2" customFormat="1" hidden="1">
       <c r="F4" s="3"/>
@@ -2820,9 +2998,9 @@
       <c r="L8" s="5"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="2:20" s="2" customFormat="1" ht="21">
+    <row r="9" spans="2:20" s="2" customFormat="1" ht="20.25">
       <c r="B9" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -2843,7 +3021,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="2:20" s="2" customFormat="1" ht="12.6" thickBot="1">
+    <row r="11" spans="2:20" s="2" customFormat="1" ht="12.75" thickBot="1">
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2864,54 +3042,54 @@
       <c r="E12" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="37" t="s">
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="31" t="s">
         <v>6</v>
       </c>
       <c r="M12" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
     </row>
     <row r="13" spans="2:20" ht="24" customHeight="1">
       <c r="B13" s="14">
-        <f t="shared" ref="B13:B32" ca="1" si="0">F13</f>
+        <f t="shared" ref="B13:B27" ca="1" si="0">F13</f>
         <v>1</v>
       </c>
       <c r="C13" s="15">
-        <f t="shared" ref="C13:C30" ca="1" si="1">IF(E13="Select","",IF(AND(F13=1,E13&lt;&gt;"Select"),$K$3,OFFSET(C13,-1,1)))</f>
+        <f t="shared" ref="C13:C26" ca="1" si="1">IF(E13="Select","",IF(AND(F13=1,E13&lt;&gt;"Select"),$K$3,OFFSET(C13,-1,1)))</f>
         <v>0.375</v>
       </c>
       <c r="D13" s="15">
-        <f t="shared" ref="D13:D30" ca="1" si="2">IF(ISERROR(E13+C13),"",E13+C13)</f>
-        <v>0.38541666666666669</v>
+        <f t="shared" ref="D13:D26" ca="1" si="2">IF(ISERROR(E13+C13),"",E13+C13)</f>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E13" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F13" s="17">
-        <f t="shared" ref="F13:F30" ca="1" si="3">ROW()-ROW(OFFSET(F13,-1,))+IF(ISERROR(OFFSET(F13,-1,)*1),0,OFFSET(F13,-1,))</f>
+        <f t="shared" ref="F13:F26" ca="1" si="3">ROW()-ROW(OFFSET(F13,-1,))+IF(ISERROR(OFFSET(F13,-1,)*1),0,OFFSET(F13,-1,))</f>
         <v>1</v>
       </c>
-      <c r="G13" s="62" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="38"/>
+      <c r="G13" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="32"/>
       <c r="M13" s="17"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="49"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="41"/>
       <c r="P13" s="22"/>
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
@@ -2925,31 +3103,31 @@
       </c>
       <c r="C14" s="15">
         <f ca="1">IF(E14="Select","",IF(AND(F14=1,E14&lt;&gt;"Select"),'Day 2'!$K$3,OFFSET(C14,-1,1)))</f>
-        <v>0.38541666666666669</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="D14" s="15">
         <f ca="1">IF(ISERROR(E14+C14),"",E14+C14)</f>
-        <v>0.39583333333333337</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E14" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="F14" s="17">
         <f ca="1">ROW()-ROW(OFFSET(F14,-1,))+IF(ISERROR(OFFSET(F14,-1,)*1),0,OFFSET(F14,-1,))</f>
         <v>2</v>
       </c>
-      <c r="G14" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="38"/>
+      <c r="G14" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="32"/>
       <c r="M14" s="17"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
@@ -2962,30 +3140,30 @@
       </c>
       <c r="C15" s="15">
         <f t="shared" ref="C15" ca="1" si="5">IF(E15="Select","",IF(AND(F15=1,E15&lt;&gt;"Select"),$K$3,OFFSET(C15,-1,1)))</f>
-        <v>0.39583333333333337</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="D15" s="15">
         <f t="shared" ref="D15" ca="1" si="6">IF(ISERROR(E15+C15),"",E15+C15)</f>
-        <v>0.40625000000000006</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="E15" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="F15" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
-      <c r="G15" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="59"/>
+      <c r="G15" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="47"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="49"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="41"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
@@ -2999,30 +3177,30 @@
       </c>
       <c r="C16" s="15">
         <f ca="1">IF(E16="Select","",IF(AND(F16=1,E16&lt;&gt;"Select"),'Day 3'!$K$3,OFFSET(C16,-1,1)))</f>
-        <v>0.40625000000000006</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="D16" s="15">
         <f ca="1">IF(ISERROR(E16+C16),"",E16+C16)</f>
-        <v>0.42708333333333337</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="E16" s="16">
-        <v>2.0833333333333332E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="F16" s="17">
         <f ca="1">ROW()-ROW(OFFSET(F16,-1,))+IF(ISERROR(OFFSET(F16,-1,)*1),0,OFFSET(F16,-1,))</f>
         <v>4</v>
       </c>
-      <c r="G16" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="31"/>
+      <c r="G16" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="27"/>
       <c r="M16" s="17"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="49"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="41"/>
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
@@ -3036,11 +3214,11 @@
       </c>
       <c r="C17" s="15">
         <f ca="1">IF(E17="Select","",IF(AND(F17=1,E17&lt;&gt;"Select"),'Day 3'!$K$3,OFFSET(C17,-1,1)))</f>
-        <v>0.42708333333333337</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="D17" s="15">
         <f ca="1">IF(ISERROR(E17+C17),"",E17+C17)</f>
-        <v>0.44791666666666669</v>
+        <v>0.47916666666666663</v>
       </c>
       <c r="E17" s="16">
         <v>2.0833333333333332E-2</v>
@@ -3049,17 +3227,17 @@
         <f ca="1">ROW()-ROW(OFFSET(F17,-1,))+IF(ISERROR(OFFSET(F17,-1,)*1),0,OFFSET(F17,-1,))</f>
         <v>5</v>
       </c>
-      <c r="G17" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="31"/>
+      <c r="G17" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="27"/>
       <c r="M17" s="17"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="49"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="41"/>
       <c r="P17" s="22"/>
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
@@ -3073,30 +3251,30 @@
       </c>
       <c r="C18" s="15">
         <f ca="1">IF(E18="Select","",IF(AND(F18=1,E18&lt;&gt;"Select"),$K$3,OFFSET(C18,-1,1)))</f>
-        <v>0.44791666666666669</v>
+        <v>0.47916666666666663</v>
       </c>
       <c r="D18" s="15">
         <f ca="1">IF(ISERROR(E18+C18),"",E18+C18)</f>
-        <v>0.45833333333333337</v>
+        <v>0.49999999999999994</v>
       </c>
       <c r="E18" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F18" s="17">
         <f ca="1">ROW()-ROW(OFFSET(F18,-1,))+IF(ISERROR(OFFSET(F18,-1,)*1),0,OFFSET(F18,-1,))</f>
         <v>6</v>
       </c>
-      <c r="G18" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="31"/>
+      <c r="G18" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="27"/>
       <c r="M18" s="17"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="49"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
       <c r="P18" s="22"/>
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
@@ -3110,30 +3288,30 @@
       </c>
       <c r="C19" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.45833333333333337</v>
+        <v>0.49999999999999994</v>
       </c>
       <c r="D19" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.47222222222222227</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E19" s="16">
-        <v>1.3888888888888888E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F19" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>7</v>
       </c>
-      <c r="G19" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="31"/>
+      <c r="G19" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="27"/>
       <c r="M19" s="17"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="49"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="41"/>
       <c r="P19" s="22"/>
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
@@ -3147,30 +3325,30 @@
       </c>
       <c r="C20" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47222222222222227</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D20" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.51041666666666674</v>
+        <v>0.5625</v>
       </c>
       <c r="E20" s="16">
-        <v>3.8194444444444441E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F20" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>8</v>
       </c>
-      <c r="G20" s="62" t="s">
-        <v>63</v>
-      </c>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="31"/>
+      <c r="G20" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="27"/>
       <c r="M20" s="17"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="49"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="41"/>
       <c r="P20" s="22"/>
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
@@ -3184,30 +3362,30 @@
       </c>
       <c r="C21" s="15">
         <f ca="1">IF(E21="Select","",IF(AND(F21=1,E21&lt;&gt;"Select"),$K$3,OFFSET(C21,-1,1)))</f>
-        <v>0.51041666666666674</v>
+        <v>0.5625</v>
       </c>
       <c r="D21" s="15">
         <f ca="1">IF(ISERROR(E21+C21),"",E21+C21)</f>
-        <v>0.5277777777777779</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="E21" s="16">
-        <v>1.7361111111111112E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F21" s="17">
         <f ca="1">ROW()-ROW(OFFSET(F21,-1,))+IF(ISERROR(OFFSET(F21,-1,)*1),0,OFFSET(F21,-1,))</f>
         <v>9</v>
       </c>
-      <c r="G21" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="31"/>
+      <c r="G21" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="27"/>
       <c r="M21" s="17"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="49"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="41"/>
       <c r="P21" s="22"/>
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
@@ -3221,30 +3399,30 @@
       </c>
       <c r="C22" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5277777777777779</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D22" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.53819444444444453</v>
+        <v>0.625</v>
       </c>
       <c r="E22" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F22" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>10</v>
       </c>
-      <c r="G22" s="62" t="s">
+      <c r="G22" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="38"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="32"/>
       <c r="M22" s="17"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="49"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="41"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="22"/>
       <c r="R22" s="22"/>
@@ -3258,30 +3436,30 @@
       </c>
       <c r="C23" s="15">
         <f ca="1">IF(E23="Select","",IF(AND(F23=1,E23&lt;&gt;"Select"),$K$3,OFFSET(C23,-1,1)))</f>
-        <v>0.53819444444444453</v>
+        <v>0.625</v>
       </c>
       <c r="D23" s="15">
         <f ca="1">IF(ISERROR(E23+C23),"",E23+C23)</f>
-        <v>0.56944444444444453</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="E23" s="16">
-        <v>3.125E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="F23" s="17">
         <f ca="1">ROW()-ROW(OFFSET(F23,-1,))+IF(ISERROR(OFFSET(F23,-1,)*1),0,OFFSET(F23,-1,))</f>
         <v>11</v>
       </c>
-      <c r="G23" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="38"/>
+      <c r="G23" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="32"/>
       <c r="M23" s="17"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="49"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
       <c r="P23" s="22"/>
       <c r="Q23" s="22"/>
       <c r="R23" s="22"/>
@@ -3295,11 +3473,11 @@
       </c>
       <c r="C24" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56944444444444453</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="D24" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.5902777777777779</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="E24" s="16">
         <v>2.0833333333333332E-2</v>
@@ -3308,17 +3486,17 @@
         <f t="shared" ca="1" si="3"/>
         <v>12</v>
       </c>
-      <c r="G24" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="38"/>
+      <c r="G24" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="32"/>
       <c r="M24" s="17"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="49"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="41"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="22"/>
       <c r="R24" s="22"/>
@@ -3332,31 +3510,31 @@
       </c>
       <c r="C25" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5902777777777779</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D25" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.61111111111111127</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="E25" s="16">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F25" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>13</v>
       </c>
-      <c r="G25" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="38"/>
+      <c r="G25" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="32"/>
       <c r="M25" s="17"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="48"/>
-      <c r="P25" s="34"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="28"/>
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="22"/>
@@ -3369,30 +3547,30 @@
       </c>
       <c r="C26" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61111111111111127</v>
+        <v>0.69444444444444442</v>
       </c>
       <c r="D26" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.63194444444444464</v>
+        <v>0.70833333333333326</v>
       </c>
       <c r="E26" s="16">
-        <v>2.0833333333333332E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="F26" s="17">
         <f t="shared" ca="1" si="3"/>
         <v>14</v>
       </c>
-      <c r="G26" s="62" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" s="63"/>
-      <c r="I26" s="63"/>
-      <c r="J26" s="63"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="38"/>
+      <c r="G26" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="32"/>
       <c r="M26" s="17"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="49"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="41"/>
       <c r="P26" s="22"/>
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
@@ -3401,256 +3579,70 @@
     </row>
     <row r="27" spans="2:20" ht="24" customHeight="1">
       <c r="B27" s="14">
-        <f ca="1">F27</f>
+        <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
       <c r="C27" s="15">
-        <f ca="1">IF(E27="Select","",IF(AND(F27=1,E27&lt;&gt;"Select"),$K$3,OFFSET(C27,-1,1)))</f>
-        <v>0.63194444444444464</v>
+        <f t="shared" ref="C27" ca="1" si="7">IF(E27="Select","",IF(AND(F27=1,E27&lt;&gt;"Select"),$K$3,OFFSET(C27,-1,1)))</f>
+        <v>0.70833333333333326</v>
       </c>
       <c r="D27" s="15">
-        <f ca="1">IF(ISERROR(E27+C27),"",E27+C27)</f>
-        <v>0.64236111111111127</v>
+        <f t="shared" ref="D27" ca="1" si="8">IF(ISERROR(E27+C27),"",E27+C27)</f>
+        <v>0.74999999999999989</v>
       </c>
       <c r="E27" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F27" s="17">
-        <f ca="1">ROW()-ROW(OFFSET(F27,-1,))+IF(ISERROR(OFFSET(F27,-1,)*1),0,OFFSET(F27,-1,))</f>
+        <f t="shared" ref="F27" ca="1" si="9">ROW()-ROW(OFFSET(F27,-1,))+IF(ISERROR(OFFSET(F27,-1,)*1),0,OFFSET(F27,-1,))</f>
         <v>15</v>
       </c>
-      <c r="G27" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="38"/>
+      <c r="G27" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="46" t="s">
+        <v>22</v>
+      </c>
       <c r="M27" s="17"/>
-      <c r="N27" s="49"/>
-      <c r="O27" s="49"/>
+      <c r="N27" s="39"/>
+      <c r="O27" s="42"/>
       <c r="P27" s="22"/>
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="22"/>
       <c r="T27" s="22"/>
     </row>
-    <row r="28" spans="2:20" ht="24" customHeight="1">
-      <c r="B28" s="14">
-        <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C28" s="15">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.64236111111111127</v>
-      </c>
-      <c r="D28" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.6527777777777779</v>
-      </c>
-      <c r="E28" s="16">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="F28" s="17">
-        <f t="shared" ca="1" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="G28" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
-    </row>
-    <row r="29" spans="2:20" ht="24" customHeight="1">
-      <c r="B29" s="14">
-        <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C29" s="15">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.6527777777777779</v>
-      </c>
-      <c r="D29" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.67361111111111127</v>
-      </c>
-      <c r="E29" s="16">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F29" s="17">
-        <f t="shared" ca="1" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="G29" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="22"/>
-      <c r="S29" s="22"/>
-      <c r="T29" s="22"/>
-    </row>
-    <row r="30" spans="2:20" ht="24" customHeight="1">
-      <c r="B30" s="14">
-        <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C30" s="15">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.67361111111111127</v>
-      </c>
-      <c r="D30" s="15">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.69791666666666685</v>
-      </c>
-      <c r="E30" s="16">
-        <v>2.4305555555555556E-2</v>
-      </c>
-      <c r="F30" s="17">
-        <f t="shared" ca="1" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="G30" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="H30" s="63"/>
-      <c r="I30" s="63"/>
-      <c r="J30" s="63"/>
-      <c r="K30" s="64"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="22"/>
-      <c r="R30" s="22"/>
-      <c r="S30" s="22"/>
-      <c r="T30" s="22"/>
-    </row>
-    <row r="31" spans="2:20" ht="24" customHeight="1">
-      <c r="B31" s="14">
-        <f t="shared" ca="1" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="C31" s="15">
-        <f t="shared" ref="C31" ca="1" si="7">IF(E31="Select","",IF(AND(F31=1,E31&lt;&gt;"Select"),$K$3,OFFSET(C31,-1,1)))</f>
-        <v>0.69791666666666685</v>
-      </c>
-      <c r="D31" s="15">
-        <f t="shared" ref="D31" ca="1" si="8">IF(ISERROR(E31+C31),"",E31+C31)</f>
-        <v>0.70833333333333348</v>
-      </c>
-      <c r="E31" s="16">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="F31" s="17">
-        <f t="shared" ref="F31:F32" ca="1" si="9">ROW()-ROW(OFFSET(F31,-1,))+IF(ISERROR(OFFSET(F31,-1,)*1),0,OFFSET(F31,-1,))</f>
-        <v>19</v>
-      </c>
-      <c r="G31" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="H31" s="63"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="63"/>
-      <c r="K31" s="64"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="22"/>
-      <c r="Q31" s="22"/>
-      <c r="R31" s="22"/>
-      <c r="S31" s="22"/>
-      <c r="T31" s="22"/>
-    </row>
-    <row r="32" spans="2:20" ht="24" customHeight="1">
-      <c r="B32" s="14">
-        <f t="shared" ca="1" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C32" s="15">
-        <f t="shared" ref="C32" ca="1" si="10">IF(E32="Select","",IF(AND(F32=1,E32&lt;&gt;"Select"),$K$3,OFFSET(C32,-1,1)))</f>
-        <v>0.70833333333333348</v>
-      </c>
-      <c r="D32" s="15">
-        <f t="shared" ref="D32" ca="1" si="11">IF(ISERROR(E32+C32),"",E32+C32)</f>
-        <v>0.75000000000000011</v>
-      </c>
-      <c r="E32" s="16">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F32" s="17">
-        <f t="shared" ca="1" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="G32" s="62" t="s">
-        <v>64</v>
-      </c>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="56" t="s">
-        <v>24</v>
-      </c>
-      <c r="M32" s="17"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="50"/>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="22"/>
-      <c r="S32" s="22"/>
-      <c r="T32" s="22"/>
-    </row>
-    <row r="33" spans="2:5" ht="22.5" customHeight="1">
-      <c r="E33" s="18">
-        <f>SUM(E13:E32)</f>
-        <v>0.37500000000000006</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="15.6">
-      <c r="B36" s="13" t="s">
+    <row r="28" spans="2:20" ht="22.5" customHeight="1">
+      <c r="E28" s="18">
+        <f>SUM(E13:E27)</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" ht="15.75">
+      <c r="B31" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="15.6">
-      <c r="C39" s="44"/>
-    </row>
-    <row r="40" spans="2:5" ht="15.6">
-      <c r="C40" s="45"/>
-    </row>
-    <row r="41" spans="2:5" ht="14.4">
-      <c r="C41" s="46"/>
+    <row r="34" spans="3:3" ht="15.75">
+      <c r="C34" s="36"/>
+    </row>
+    <row r="35" spans="3:3" ht="15.75">
+      <c r="C35" s="37"/>
+    </row>
+    <row r="36" spans="3:3" ht="15">
+      <c r="C36" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="G32:K32"/>
+  <mergeCells count="18">
     <mergeCell ref="G27:K27"/>
-    <mergeCell ref="G31:K31"/>
-    <mergeCell ref="G30:K30"/>
     <mergeCell ref="G23:K23"/>
     <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G25:K25"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="G22:K22"/>
     <mergeCell ref="G20:K20"/>
@@ -3660,15 +3652,19 @@
     <mergeCell ref="G17:K17"/>
     <mergeCell ref="G14:K14"/>
     <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G21:K21"/>
   </mergeCells>
-  <conditionalFormatting sqref="E33">
+  <conditionalFormatting sqref="E28">
     <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>#REF!&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter time as H:MM:SS (update AM/PM as necessary)." sqref="K3:L11" xr:uid="{DE1472D6-3EAB-4DEA-B196-E92D7498673C}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23:E32 E13:E22" xr:uid="{BA96F81D-030C-4515-9007-019502212301}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E27" xr:uid="{BA96F81D-030C-4515-9007-019502212301}">
       <formula1>"0:00, 0:05, 0:10, 0:15, 0:20, 0:25, 0:30, 0:35, 0:40, 0:45, 0:50, 0:55, 1:00, 1:15, 1:30"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3684,27 +3680,27 @@
   </sheetPr>
   <dimension ref="B1:T37"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B27" sqref="A27:XFD27"/>
+    <sheetView topLeftCell="B11" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="2.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="2.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="14" max="251" width="9.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
+    <col min="14" max="251" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" s="1" customFormat="1" ht="14.4" hidden="1">
+    <row r="1" spans="2:20" s="1" customFormat="1" ht="15" hidden="1">
       <c r="G1" s="10" t="s">
         <v>0</v>
       </c>
@@ -3717,25 +3713,25 @@
     </row>
     <row r="2" spans="2:20" ht="12" hidden="1" customHeight="1">
       <c r="E2" s="12"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="42"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="2:20" ht="12" hidden="1" customHeight="1">
       <c r="E3" s="12"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="8"/>
       <c r="K3" s="9">
         <v>0.375</v>
@@ -3743,7 +3739,7 @@
       <c r="L3" s="9">
         <v>0.70833333333333337</v>
       </c>
-      <c r="M3" s="36"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="2:20" s="2" customFormat="1" hidden="1">
       <c r="F4" s="3"/>
@@ -3795,9 +3791,9 @@
       <c r="L8" s="5"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="2:20" s="2" customFormat="1" ht="21">
+    <row r="9" spans="2:20" s="2" customFormat="1" ht="20.25">
       <c r="B9" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -3818,7 +3814,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="2:20" s="2" customFormat="1" ht="12.6" thickBot="1">
+    <row r="11" spans="2:20" s="2" customFormat="1" ht="12.75" thickBot="1">
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -3839,22 +3835,22 @@
       <c r="E12" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="43" t="s">
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="35" t="s">
         <v>6</v>
       </c>
       <c r="M12" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
     </row>
     <row r="13" spans="2:20" ht="24" customHeight="1">
       <c r="B13" s="14">
@@ -3867,26 +3863,26 @@
       </c>
       <c r="D13" s="15">
         <f ca="1">IF(ISERROR(E13+C13),"",E13+C13)</f>
-        <v>0.38541666666666669</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E13" s="16">
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F13" s="17">
         <f t="shared" ref="F13:F22" ca="1" si="0">ROW()-ROW(OFFSET(F13,-1,))+IF(ISERROR(OFFSET(F13,-1,)*1),0,OFFSET(F13,-1,))</f>
         <v>1</v>
       </c>
-      <c r="G13" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="39"/>
+      <c r="G13" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="33"/>
       <c r="M13" s="17"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="49"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="41"/>
       <c r="P13" s="22"/>
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
@@ -3900,30 +3896,30 @@
       </c>
       <c r="C14" s="15">
         <f ca="1">IF(E14="Select","",IF(AND(F14=1,E14&lt;&gt;"Select"),$K$3,OFFSET(C14,-1,1)))</f>
-        <v>0.38541666666666669</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="D14" s="15">
         <f ca="1">IF(ISERROR(E14+C14),"",E14+C14)</f>
-        <v>0.4375</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="E14" s="16">
-        <v>5.2083333333333336E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F14" s="17">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="G14" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="60"/>
+      <c r="G14" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="48"/>
       <c r="M14" s="17"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="49"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="41"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
@@ -3937,11 +3933,11 @@
       </c>
       <c r="C15" s="15">
         <f ca="1">IF(E15="Select","",IF(AND(F15=1,E15&lt;&gt;"Select"),$K$3,OFFSET(C15,-1,1)))</f>
-        <v>0.4375</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="D15" s="15">
         <f ca="1">IF(ISERROR(E15+C15),"",E15+C15)</f>
-        <v>0.44791666666666669</v>
+        <v>0.42708333333333331</v>
       </c>
       <c r="E15" s="16">
         <v>1.0416666666666666E-2</v>
@@ -3950,17 +3946,17 @@
         <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="G15" s="62" t="s">
+      <c r="G15" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="61"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="49"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="49"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="41"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
@@ -3974,11 +3970,11 @@
       </c>
       <c r="C16" s="15">
         <f t="shared" ref="C16:C21" ca="1" si="2">IF(E16="Select","",IF(AND(F16=1,E16&lt;&gt;"Select"),$K$3,OFFSET(C16,-1,1)))</f>
-        <v>0.44791666666666669</v>
+        <v>0.42708333333333331</v>
       </c>
       <c r="D16" s="15">
         <f t="shared" ref="D16:D21" ca="1" si="3">IF(ISERROR(E16+C16),"",E16+C16)</f>
-        <v>0.46875</v>
+        <v>0.44791666666666663</v>
       </c>
       <c r="E16" s="16">
         <v>2.0833333333333332E-2</v>
@@ -3987,17 +3983,17 @@
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="G16" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="39"/>
+      <c r="G16" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="33"/>
       <c r="M16" s="17"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="49"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="41"/>
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
@@ -4011,11 +4007,11 @@
       </c>
       <c r="C17" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.46875</v>
+        <v>0.44791666666666663</v>
       </c>
       <c r="D17" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.52083333333333337</v>
+        <v>0.49999999999999994</v>
       </c>
       <c r="E17" s="16">
         <v>5.2083333333333336E-2</v>
@@ -4024,17 +4020,17 @@
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="G17" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="39"/>
+      <c r="G17" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="33"/>
       <c r="M17" s="17"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="49"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
       <c r="P17" s="22"/>
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
@@ -4048,11 +4044,11 @@
       </c>
       <c r="C18" s="15">
         <f ca="1">IF(E18="Select","",IF(AND(F18=1,E18&lt;&gt;"Select"),$K$3,OFFSET(C18,-1,1)))</f>
-        <v>0.52083333333333337</v>
+        <v>0.49999999999999994</v>
       </c>
       <c r="D18" s="15">
         <f ca="1">IF(ISERROR(E18+C18),"",E18+C18)</f>
-        <v>0.5625</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E18" s="16">
         <v>4.1666666666666664E-2</v>
@@ -4061,17 +4057,17 @@
         <f ca="1">ROW()-ROW(OFFSET(F18,-1,))+IF(ISERROR(OFFSET(F18,-1,)*1),0,OFFSET(F18,-1,))</f>
         <v>6</v>
       </c>
-      <c r="G18" s="62" t="s">
+      <c r="G18" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="39"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="33"/>
       <c r="M18" s="17"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="49"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
       <c r="P18" s="22"/>
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
@@ -4085,11 +4081,11 @@
       </c>
       <c r="C19" s="15">
         <f ca="1">IF(E19="Select","",IF(AND(F19=1,E19&lt;&gt;"Select"),$K$3,OFFSET(C19,-1,1)))</f>
-        <v>0.5625</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D19" s="15">
         <f ca="1">IF(ISERROR(E19+C19),"",E19+C19)</f>
-        <v>0.57291666666666663</v>
+        <v>0.55208333333333326</v>
       </c>
       <c r="E19" s="16">
         <v>1.0416666666666666E-2</v>
@@ -4098,18 +4094,18 @@
         <f ca="1">ROW()-ROW(OFFSET(F19,-1,))+IF(ISERROR(OFFSET(F19,-1,)*1),0,OFFSET(F19,-1,))</f>
         <v>7</v>
       </c>
-      <c r="G19" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="39"/>
+      <c r="G19" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="33"/>
       <c r="M19" s="17"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="34"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="28"/>
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
@@ -4122,11 +4118,11 @@
       </c>
       <c r="C20" s="15">
         <f ca="1">IF(E20="Select","",IF(AND(F20=1,E20&lt;&gt;"Select"),$K$3,OFFSET(C20,-1,1)))</f>
-        <v>0.57291666666666663</v>
+        <v>0.55208333333333326</v>
       </c>
       <c r="D20" s="15">
         <f ca="1">IF(ISERROR(E20+C20),"",E20+C20)</f>
-        <v>0.59375</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="E20" s="16">
         <v>2.0833333333333332E-2</v>
@@ -4135,17 +4131,17 @@
         <f ca="1">ROW()-ROW(OFFSET(F20,-1,))+IF(ISERROR(OFFSET(F20,-1,)*1),0,OFFSET(F20,-1,))</f>
         <v>8</v>
       </c>
-      <c r="G20" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="39"/>
+      <c r="G20" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="33"/>
       <c r="M20" s="17"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="49"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="41"/>
       <c r="P20" s="22"/>
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
@@ -4159,11 +4155,11 @@
       </c>
       <c r="C21" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.59375</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="D21" s="15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.60416666666666663</v>
+        <v>0.58333333333333326</v>
       </c>
       <c r="E21" s="16">
         <v>1.0416666666666666E-2</v>
@@ -4172,17 +4168,17 @@
         <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
-      <c r="G21" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="39"/>
+      <c r="G21" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="33"/>
       <c r="M21" s="17"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="49"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="41"/>
       <c r="P21" s="22"/>
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
@@ -4196,11 +4192,11 @@
       </c>
       <c r="C22" s="15">
         <f t="shared" ref="C22" ca="1" si="5">IF(E22="Select","",IF(AND(F22=1,E22&lt;&gt;"Select"),$K$3,OFFSET(C22,-1,1)))</f>
-        <v>0.60416666666666663</v>
+        <v>0.58333333333333326</v>
       </c>
       <c r="D22" s="15">
         <f t="shared" ref="D22" ca="1" si="6">IF(ISERROR(E22+C22),"",E22+C22)</f>
-        <v>0.625</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="E22" s="16">
         <v>2.0833333333333332E-2</v>
@@ -4209,17 +4205,17 @@
         <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
-      <c r="G22" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="39"/>
+      <c r="G22" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="33"/>
       <c r="M22" s="17"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="49"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="41"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="22"/>
       <c r="R22" s="22"/>
@@ -4233,11 +4229,11 @@
       </c>
       <c r="C23" s="15">
         <f t="shared" ref="C23:C28" ca="1" si="7">IF(E23="Select","",IF(AND(F23=1,E23&lt;&gt;"Select"),$K$3,OFFSET(C23,-1,1)))</f>
-        <v>0.625</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D23" s="15">
         <f t="shared" ref="D23:D28" ca="1" si="8">IF(ISERROR(E23+C23),"",E23+C23)</f>
-        <v>0.63541666666666663</v>
+        <v>0.61458333333333326</v>
       </c>
       <c r="E23" s="16">
         <v>1.0416666666666666E-2</v>
@@ -4246,17 +4242,17 @@
         <f t="shared" ref="F23:F28" ca="1" si="9">ROW()-ROW(OFFSET(F23,-1,))+IF(ISERROR(OFFSET(F23,-1,)*1),0,OFFSET(F23,-1,))</f>
         <v>11</v>
       </c>
-      <c r="G23" s="62" t="s">
+      <c r="G23" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="39"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="33"/>
       <c r="M23" s="17"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="49"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
       <c r="P23" s="22"/>
       <c r="Q23" s="22"/>
       <c r="R23" s="22"/>
@@ -4270,11 +4266,11 @@
       </c>
       <c r="C24" s="15">
         <f t="shared" ca="1" si="7"/>
-        <v>0.63541666666666663</v>
+        <v>0.61458333333333326</v>
       </c>
       <c r="D24" s="15">
         <f t="shared" ca="1" si="8"/>
-        <v>0.65625</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="E24" s="16">
         <v>2.0833333333333332E-2</v>
@@ -4283,17 +4279,17 @@
         <f t="shared" ca="1" si="9"/>
         <v>12</v>
       </c>
-      <c r="G24" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="39"/>
+      <c r="G24" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="33"/>
       <c r="M24" s="17"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="22"/>
       <c r="R24" s="22"/>
@@ -4307,11 +4303,11 @@
       </c>
       <c r="C25" s="15">
         <f t="shared" ca="1" si="7"/>
-        <v>0.65625</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="D25" s="15">
         <f t="shared" ca="1" si="8"/>
-        <v>0.65625</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="E25" s="16">
         <v>0</v>
@@ -4320,17 +4316,17 @@
         <f t="shared" ca="1" si="9"/>
         <v>13</v>
       </c>
-      <c r="G25" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="H25" s="63"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="63"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="39"/>
+      <c r="G25" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="33"/>
       <c r="M25" s="17"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="49"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="41"/>
       <c r="P25" s="22"/>
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
@@ -4344,11 +4340,11 @@
       </c>
       <c r="C26" s="15">
         <f t="shared" ca="1" si="7"/>
-        <v>0.65625</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="D26" s="15">
         <f t="shared" ca="1" si="8"/>
-        <v>0.6875</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E26" s="16">
         <v>3.125E-2</v>
@@ -4357,19 +4353,19 @@
         <f t="shared" ca="1" si="9"/>
         <v>14</v>
       </c>
-      <c r="G26" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="63"/>
-      <c r="I26" s="63"/>
-      <c r="J26" s="63"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="39" t="s">
-        <v>24</v>
+      <c r="G26" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="33" t="s">
+        <v>22</v>
       </c>
       <c r="M26" s="17"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="49"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="41"/>
       <c r="P26" s="22"/>
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
@@ -4383,11 +4379,11 @@
       </c>
       <c r="C27" s="15">
         <f t="shared" ca="1" si="7"/>
-        <v>0.6875</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D27" s="15">
         <f t="shared" ca="1" si="8"/>
-        <v>0.70833333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="E27" s="16">
         <v>2.0833333333333332E-2</v>
@@ -4396,17 +4392,17 @@
         <f t="shared" ca="1" si="9"/>
         <v>15</v>
       </c>
-      <c r="G27" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="60"/>
+      <c r="G27" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="48"/>
       <c r="M27" s="17"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="49"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="41"/>
       <c r="P27" s="22"/>
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
@@ -4420,11 +4416,11 @@
       </c>
       <c r="C28" s="15">
         <f t="shared" ca="1" si="7"/>
-        <v>0.70833333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="D28" s="15">
         <f t="shared" ca="1" si="8"/>
-        <v>0.72916666666666674</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="E28" s="16">
         <v>2.0833333333333332E-2</v>
@@ -4433,19 +4429,19 @@
         <f t="shared" ca="1" si="9"/>
         <v>16</v>
       </c>
-      <c r="G28" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28" s="63"/>
-      <c r="I28" s="63"/>
-      <c r="J28" s="63"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="56" t="s">
-        <v>24</v>
+      <c r="G28" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="46" t="s">
+        <v>22</v>
       </c>
       <c r="M28" s="17"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="49"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="41"/>
       <c r="P28" s="22"/>
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
@@ -4455,39 +4451,44 @@
     <row r="29" spans="2:20" ht="22.5" customHeight="1">
       <c r="E29" s="18">
         <f>SUM(E13:E28)</f>
-        <v>0.35416666666666663</v>
-      </c>
-    </row>
-    <row r="32" spans="2:20" ht="15.6">
+        <v>0.33333333333333326</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" ht="15.75">
       <c r="B32" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="3:3" ht="15.6">
-      <c r="C35" s="44"/>
-    </row>
-    <row r="36" spans="3:3" ht="15.6">
-      <c r="C36" s="45"/>
-    </row>
-    <row r="37" spans="3:3" ht="14.4">
-      <c r="C37" s="46"/>
+    <row r="35" spans="3:3" ht="15.75">
+      <c r="C35" s="36"/>
+    </row>
+    <row r="36" spans="3:3" ht="15.75">
+      <c r="C36" s="37"/>
+    </row>
+    <row r="37" spans="3:3" ht="15">
+      <c r="C37" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="G26:K26"/>
+  <mergeCells count="19">
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G27:K27"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="F12:K12"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="G16:K16"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G15:K15"/>
     <mergeCell ref="G14:K14"/>
-    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="G26:K26"/>
   </mergeCells>
   <conditionalFormatting sqref="E29">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">

</xml_diff>